<commit_message>
added sum command (adds total sales)
</commit_message>
<xml_diff>
--- a/data/expenditure.xlsx
+++ b/data/expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0acdd9fbc4c9e779/Documents/GitHub/Expenditure_Tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{48F7D44C-6659-4B7C-BBC3-1A5C7D9706A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{48F7D44C-6659-4B7C-BBC3-1A5C7D9706A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B293EB8B-1951-49A9-9524-75D96B2F6BCD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -421,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +432,7 @@
     <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -450,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -468,7 +467,7 @@
         <v>18.72298</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -486,7 +485,7 @@
         <v>6.6120000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -503,8 +502,9 @@
         <f t="shared" si="0"/>
         <v>6.2703800000000012</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -522,7 +522,7 @@
         <v>13.224970000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -540,7 +540,7 @@
         <v>50.669960000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -558,7 +558,7 @@
         <v>4.396980000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -576,7 +576,7 @@
         <v>4.396980000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -594,7 +594,7 @@
         <v>22.048969999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -612,7 +612,7 @@
         <v>15.416980000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -630,7 +630,7 @@
         <v>13.212980000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>

</xml_diff>